<commit_message>
Fixed some bugs in auditing
</commit_message>
<xml_diff>
--- a/Excel/Atualização/Atividades/Atividades.xlsx
+++ b/Excel/Atualização/Atividades/Atividades.xlsx
@@ -20,15 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t xml:space="preserve">Vídeoaula no youtube sobre conjuntos numéricos.</t>
+    <t xml:space="preserve">Atividade01_atualizado</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.youtube.com/watch?v=JHcFDgsLvlo</t>
+    <t xml:space="preserve">Atividade02_atualizado</t>
   </si>
   <si>
-    <t xml:space="preserve">Vídeoaula no youtube sobre acentuação</t>
+    <t xml:space="preserve">Atividade03_atualizado</t>
   </si>
 </sst>
 </file>
@@ -104,17 +104,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -134,38 +138,43 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="69.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
-        <v>157045</v>
+        <v>158070</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>157046</v>
+        <v>158071</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>158072</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>